<commit_message>
manh hop dong gia han
</commit_message>
<xml_diff>
--- a/xuattttt.xlsx
+++ b/xuattttt.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>STT</t>
   </si>
@@ -41,52 +41,25 @@
     <t>Tình trạng</t>
   </si>
   <si>
-    <t>nv2</t>
-  </si>
-  <si>
-    <t>sv1</t>
-  </si>
-  <si>
-    <t>102A1</t>
-  </si>
-  <si>
-    <t>2024-06-08</t>
+    <t>HD1</t>
+  </si>
+  <si>
+    <t>NV005</t>
+  </si>
+  <si>
+    <t>SV005</t>
+  </si>
+  <si>
+    <t>A101</t>
   </si>
   <si>
     <t>2024-06-24</t>
   </si>
   <si>
+    <t>2024-06-26</t>
+  </si>
+  <si>
     <t>Hết hạn</t>
-  </si>
-  <si>
-    <t>hd2</t>
-  </si>
-  <si>
-    <t>sv2</t>
-  </si>
-  <si>
-    <t>2024-06-21</t>
-  </si>
-  <si>
-    <t>Còn hạn</t>
-  </si>
-  <si>
-    <t>hd3</t>
-  </si>
-  <si>
-    <t>nv1</t>
-  </si>
-  <si>
-    <t>sv3</t>
-  </si>
-  <si>
-    <t>103A1</t>
-  </si>
-  <si>
-    <t>2024-06-05</t>
-  </si>
-  <si>
-    <t>2024-06-26</t>
   </si>
 </sst>
 </file>
@@ -463,7 +436,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -511,78 +484,26 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>